<commit_message>
fixed log diff bug in panelSVAR
</commit_message>
<xml_diff>
--- a/lambda-matrices.xlsx
+++ b/lambda-matrices.xlsx
@@ -460,7 +460,7 @@
         <v>112</v>
       </c>
       <c r="B2" t="n">
-        <v>-8.056006852267327e-17</v>
+        <v>0.0005881046711928496</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2.838909004359079e-16</v>
+        <v>-5.964865894906583e-06</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         <v>124</v>
       </c>
       <c r="B3" t="n">
-        <v>1.285548918456466e-17</v>
+        <v>0.0007106762814854439</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -486,7 +486,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>2.991293011692155e-17</v>
+        <v>3.436732447910796e-05</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +494,7 @@
         <v>128</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.267655801306882e-16</v>
+        <v>0.0006335075845851586</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -503,7 +503,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>2.257977135645865e-16</v>
+        <v>-3.630525363082219e-05</v>
       </c>
     </row>
     <row r="5">
@@ -511,7 +511,7 @@
         <v>132</v>
       </c>
       <c r="B5" t="n">
-        <v>-9.351387069254701e-17</v>
+        <v>0.0006615361256894055</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -520,7 +520,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1.373218166923818e-16</v>
+        <v>4.274663599907008e-06</v>
       </c>
     </row>
     <row r="6">
@@ -528,7 +528,7 @@
         <v>134</v>
       </c>
       <c r="B6" t="n">
-        <v>1.844629325035953e-17</v>
+        <v>0.0006915173597617815</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -537,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.419539942619617e-17</v>
+        <v>6.546784146951276e-06</v>
       </c>
     </row>
     <row r="7">
@@ -545,7 +545,7 @@
         <v>136</v>
       </c>
       <c r="B7" t="n">
-        <v>-2.444702370502612e-15</v>
+        <v>0.0006078264176520566</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -554,7 +554,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>4.585853885073424e-15</v>
+        <v>6.911221568933375e-06</v>
       </c>
     </row>
     <row r="8">
@@ -562,7 +562,7 @@
         <v>138</v>
       </c>
       <c r="B8" t="n">
-        <v>9.807291791923797e-17</v>
+        <v>0.0007025410390505877</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -571,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.301963151349307e-16</v>
+        <v>2.081241962251094e-05</v>
       </c>
     </row>
     <row r="9">
@@ -579,7 +579,7 @@
         <v>144</v>
       </c>
       <c r="B9" t="n">
-        <v>-4.224276307600718e-16</v>
+        <v>0.0005667850321242321</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -588,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>3.510506518271516e-16</v>
+        <v>4.966710041345766e-05</v>
       </c>
     </row>
     <row r="10">
@@ -596,7 +596,7 @@
         <v>146</v>
       </c>
       <c r="B10" t="n">
-        <v>5.269863961424123e-17</v>
+        <v>0.0007249076506473078</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -605,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>-9.030201937757984e-17</v>
+        <v>1.688198020020902e-05</v>
       </c>
     </row>
     <row r="11">
@@ -613,7 +613,7 @@
         <v>156</v>
       </c>
       <c r="B11" t="n">
-        <v>-5.835107245680767e-18</v>
+        <v>5.128518390587353e-05</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -622,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>2.795231550367543e-18</v>
+        <v>1.037262980730099e-05</v>
       </c>
     </row>
     <row r="12">
@@ -630,7 +630,7 @@
         <v>158</v>
       </c>
       <c r="B12" t="n">
-        <v>3.300882268793903e-16</v>
+        <v>0.0004169920693194457</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -639,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>-3.929805670072085e-16</v>
+        <v>-4.469129283828405e-05</v>
       </c>
     </row>
     <row r="13">
@@ -647,7 +647,7 @@
         <v>174</v>
       </c>
       <c r="B13" t="n">
-        <v>3.068185548264719e-17</v>
+        <v>0.0004762908146186371</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -656,7 +656,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1.667753823857961e-15</v>
+        <v>0.000136602067550312</v>
       </c>
     </row>
     <row r="14">
@@ -664,7 +664,7 @@
         <v>182</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.627060926402222e-16</v>
+        <v>0.0006145257326382552</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -673,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>6.12990632380922e-16</v>
+        <v>2.714017044654308e-05</v>
       </c>
     </row>
     <row r="15">
@@ -681,7 +681,7 @@
         <v>184</v>
       </c>
       <c r="B15" t="n">
-        <v>-2.671408185246545e-17</v>
+        <v>0.0005703796024620223</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>6.155400064234358e-16</v>
+        <v>9.271446636989776e-05</v>
       </c>
     </row>
     <row r="16">
@@ -698,7 +698,7 @@
         <v>186</v>
       </c>
       <c r="B16" t="n">
-        <v>1.854800402491824e-14</v>
+        <v>0.0003569228620256335</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>-6.59670468538097e-15</v>
+        <v>5.698415902919256e-05</v>
       </c>
     </row>
     <row r="17">
@@ -715,7 +715,7 @@
         <v>199</v>
       </c>
       <c r="B17" t="n">
-        <v>-9.05489846265704e-17</v>
+        <v>-0.0002789815570912871</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -724,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.823267989564459e-16</v>
+        <v>9.577714406706785e-05</v>
       </c>
     </row>
     <row r="18">
@@ -732,7 +732,7 @@
         <v>228</v>
       </c>
       <c r="B18" t="n">
-        <v>-1.408627330224587e-15</v>
+        <v>5.628193033144896e-18</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -741,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>8.397510003526347e-16</v>
+        <v>-6.570194726900558e-17</v>
       </c>
     </row>
     <row r="19">
@@ -749,7 +749,7 @@
         <v>273</v>
       </c>
       <c r="B19" t="n">
-        <v>-2.434777050345813e-05</v>
+        <v>9.533163131658903e-05</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>3.546890665775901e-05</v>
+        <v>9.976337117248558e-05</v>
       </c>
     </row>
     <row r="20">
@@ -766,7 +766,7 @@
         <v>534</v>
       </c>
       <c r="B20" t="n">
-        <v>5.986493777830897e-17</v>
+        <v>0.0001799581975221381</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -775,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>6.537792830134283e-17</v>
+        <v>6.013161025933823e-05</v>
       </c>
     </row>
     <row r="21">
@@ -783,7 +783,7 @@
         <v>542</v>
       </c>
       <c r="B21" t="n">
-        <v>0.007728667459331824</v>
+        <v>-2.715287970367651e-16</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -792,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.001559687953522578</v>
+        <v>1.61984559752848e-16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug in covariance mat in shortAndLong
</commit_message>
<xml_diff>
--- a/lambda-matrices.xlsx
+++ b/lambda-matrices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,11 +456,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>112</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0005881046711928496</v>
+        <v>0.003594426707676007</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -469,15 +471,17 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-5.964865894906583e-06</v>
+        <v>0.00335752130000186</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>124</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Russia</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0007106762814854439</v>
+        <v>-0.08937764763238913</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -486,15 +490,17 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>3.436732447910796e-05</v>
+        <v>0.01776197274421594</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>128</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Croatia</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0006335075845851586</v>
+        <v>-0.1276816929665264</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -503,15 +509,17 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-3.630525363082219e-05</v>
+        <v>-0.02151266644149382</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>132</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Belarus</t>
+        </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0006615361256894055</v>
+        <v>-0.08559797249760843</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -520,15 +528,17 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>4.274663599907008e-06</v>
+        <v>-0.01732595590511024</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>134</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0006915173597617815</v>
+        <v>-0.0910448767946363</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -537,15 +547,17 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>6.546784146951276e-06</v>
+        <v>0.03974658197051483</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>136</v>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0006078264176520566</v>
+        <v>-0.07277416962029694</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -554,15 +566,17 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>6.911221568933375e-06</v>
+        <v>-0.004865639956500455</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>138</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0007025410390505877</v>
+        <v>-0.1487620386313794</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -571,15 +585,17 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>2.081241962251094e-05</v>
+        <v>-0.0125790559403589</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>144</v>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Brazil</t>
+        </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0005667850321242321</v>
+        <v>-0.05243371295263715</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -588,15 +604,17 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>4.966710041345766e-05</v>
+        <v>0.006774072014952683</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>146</v>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>CostaRica</t>
+        </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0007249076506473078</v>
+        <v>-0.034306911320214</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -605,15 +623,17 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1.688198020020902e-05</v>
+        <v>-0.01446571529172644</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>156</v>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Lithuania</t>
+        </is>
       </c>
       <c r="B11" t="n">
-        <v>5.128518390587353e-05</v>
+        <v>-0.09808361481614002</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -622,15 +642,17 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>1.037262980730099e-05</v>
+        <v>0.01391181470309711</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>158</v>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>NewZealand</t>
+        </is>
       </c>
       <c r="B12" t="n">
-        <v>0.0004169920693194457</v>
+        <v>-0.03571315012983653</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -639,15 +661,17 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>-4.469129283828405e-05</v>
+        <v>-0.01015458080449878</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>174</v>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Peru</t>
+        </is>
       </c>
       <c r="B13" t="n">
-        <v>0.0004762908146186371</v>
+        <v>4.184127363048948e-15</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -656,15 +680,17 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.000136602067550312</v>
+        <v>-5.642384826947066e-15</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>182</v>
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>SouthAfrica</t>
+        </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0006145257326382552</v>
+        <v>0.006166357788093623</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -673,15 +699,17 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>2.714017044654308e-05</v>
+        <v>0.006505781502471442</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>184</v>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
       </c>
       <c r="B15" t="n">
-        <v>0.0005703796024620223</v>
+        <v>-0.06644222053229905</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -690,15 +718,17 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>9.271446636989776e-05</v>
+        <v>-0.01754288070602657</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>186</v>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Bulgaria</t>
+        </is>
       </c>
       <c r="B16" t="n">
-        <v>0.0003569228620256335</v>
+        <v>-0.09779532923382694</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -707,15 +737,17 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>5.698415902919256e-05</v>
+        <v>0.02108181395342322</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>199</v>
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.0002789815570912871</v>
+        <v>0.008566525556498528</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -724,15 +756,17 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>9.577714406706785e-05</v>
+        <v>-0.03061231077636284</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>228</v>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Colombia</t>
+        </is>
       </c>
       <c r="B18" t="n">
-        <v>5.628193033144896e-18</v>
+        <v>-0.1058346179478553</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -741,15 +775,17 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>-6.570194726900558e-17</v>
+        <v>-0.01088195249482424</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>273</v>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
       </c>
       <c r="B19" t="n">
-        <v>9.533163131658903e-05</v>
+        <v>-0.097364534278854</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -758,42 +794,15 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>9.976337117248558e-05</v>
+        <v>0.02225770229213496</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>534</v>
-      </c>
-      <c r="B20" t="n">
-        <v>0.0001799581975221381</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>6.013161025933823e-05</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>542</v>
-      </c>
-      <c r="B21" t="n">
-        <v>-2.715287970367651e-16</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1.61984559752848e-16</v>
-      </c>
+      <c r="A20" s="1" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
bug correction (lin.intercept) in panelSVAR
</commit_message>
<xml_diff>
--- a/lambda-matrices.xlsx
+++ b/lambda-matrices.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Lambda11</t>
   </si>
@@ -22,25 +22,10 @@
     <t>Lambda12</t>
   </si>
   <si>
-    <t>Lambda13</t>
-  </si>
-  <si>
     <t>Lambda21</t>
   </si>
   <si>
     <t>Lambda22</t>
-  </si>
-  <si>
-    <t>Lambda23</t>
-  </si>
-  <si>
-    <t>Lambda31</t>
-  </si>
-  <si>
-    <t>Lambda32</t>
-  </si>
-  <si>
-    <t>Lambda33</t>
   </si>
 </sst>
 </file>
@@ -398,13 +383,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,28 +402,13 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>112</v>
       </c>
       <c r="B2">
-        <v>-0.005508179354291032</v>
+        <v>1.230889851801546</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -447,30 +417,15 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0.008938460476857717</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>-0.004309799028655069</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>0.8071883178891555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>124</v>
       </c>
       <c r="B3">
-        <v>2.077945015202262E-16</v>
+        <v>1.475794676328668</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -479,30 +434,15 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>-5.176109843769765E-16</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>-1.103519784818E-15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>1.089242729315534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>128</v>
       </c>
       <c r="B4">
-        <v>-0.006487801449886688</v>
+        <v>1.379480861910617</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -511,30 +451,15 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0.006795598120391681</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>-0.0203576723015802</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>1.103624332836462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>132</v>
       </c>
       <c r="B5">
-        <v>0.0009373174092421929</v>
+        <v>1.409492648720695</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -543,30 +468,15 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0.002489378151065321</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>-0.01537147889855012</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>1.097746114206261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>134</v>
       </c>
       <c r="B6">
-        <v>-0.01412358875715773</v>
+        <v>1.44878911943862</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -575,30 +485,15 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0.00398680190628317</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>-0.07656865569631574</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>1.128472255581805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>136</v>
       </c>
       <c r="B7">
-        <v>0.001981782728598053</v>
+        <v>1.247436553938551</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -607,30 +502,15 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0.001454036600171476</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>-0.149352412211009</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>0.946256301812524</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>138</v>
       </c>
       <c r="B8">
-        <v>0.002371789656287733</v>
+        <v>1.456552502011144</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -639,30 +519,15 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0.01091566422381312</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0.03180573553790194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>1.096679751589838</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>144</v>
       </c>
       <c r="B9">
-        <v>-0.006896732328718494</v>
+        <v>1.138840326809303</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -671,30 +536,15 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0.0003918951100071941</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>-0.1277504178693311</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>0.8146709744382992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>146</v>
       </c>
       <c r="B10">
-        <v>-0.01638004879947816</v>
+        <v>1.494703694281028</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -703,30 +553,15 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0.01501965087481797</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0.1338929147212828</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>1.150868564405711</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>156</v>
       </c>
       <c r="B11">
-        <v>-0.0004725126586532698</v>
+        <v>0.1210644366804533</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -735,30 +570,15 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>-0.0005548522274354051</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>-0.05920408303099291</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>0.06957550961839352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>158</v>
       </c>
       <c r="B12">
-        <v>0.002041595929162186</v>
+        <v>0.9343045444177912</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -767,30 +587,15 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0.00370189070163227</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0.1920948317551884</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>0.7273558831752406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>174</v>
       </c>
       <c r="B13">
-        <v>1.347576413712589E-15</v>
+        <v>0.9376709675144884</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -799,30 +604,15 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>-2.074079192025494E-15</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>3.097083142221761E-14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>0.7418794033741131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>182</v>
       </c>
       <c r="B14">
-        <v>-0.003226672394457457</v>
+        <v>1.293877738442294</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -831,30 +621,15 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0.000541924512858556</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>-0.1332570968819717</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>0.9433595633217612</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>184</v>
       </c>
       <c r="B15">
-        <v>0.0002881308701940611</v>
+        <v>1.166734449389536</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -863,30 +638,15 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0.01515125441423137</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0.112979155436787</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>0.850607070657737</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>186</v>
       </c>
       <c r="B16">
-        <v>-1.658796118698763E-15</v>
+        <v>0.7436178228027602</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -895,30 +655,15 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>1.099001315213126E-14</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>1.286112201032636E-13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>0.6627016118747427</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>199</v>
       </c>
       <c r="B17">
-        <v>0.002592614694060558</v>
+        <v>0.617090868160048</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -927,30 +672,15 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0.0002500142511726423</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>-0.1398838091147591</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>0.3938635123240491</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>228</v>
       </c>
       <c r="B18">
-        <v>-2.340028616434546E-14</v>
+        <v>0.2422080669054435</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -959,30 +689,15 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>9.479750930291516E-14</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>1.464907495278339E-12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>0.1356000331051816</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>273</v>
       </c>
       <c r="B19">
-        <v>-3.875351624148929E-15</v>
+        <v>0.1641790834795318</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -991,30 +706,15 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>4.266229766623282E-15</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>2.401956414802682E-13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>1.737919168122043</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>534</v>
       </c>
       <c r="B20">
-        <v>-0.003051732710890893</v>
+        <v>0.4376019730568618</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1023,30 +723,15 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0.002562916707434787</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>-0.09301567353559693</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>0.5239851932030828</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>542</v>
       </c>
       <c r="B21">
-        <v>0.000861284204541108</v>
+        <v>0.1052137475793599</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1055,22 +740,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0.0005282684751840935</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>-0.1629014581460173</v>
+        <v>0.05594582501160034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction of shock normalization in shortAndLong
</commit_message>
<xml_diff>
--- a/lambda-matrices.xlsx
+++ b/lambda-matrices.xlsx
@@ -438,7 +438,7 @@
         <v>112</v>
       </c>
       <c r="B2">
-        <v>0.6211653795948238</v>
+        <v>0.7104350185607621</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.02151043289211089</v>
+        <v>0.4741996535665807</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>-0.363487266002584</v>
+        <v>-0.6365504684646589</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -470,7 +470,7 @@
         <v>124</v>
       </c>
       <c r="B3">
-        <v>0.8702544070077788</v>
+        <v>0.8813651726852317</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>-0.05553089563036782</v>
+        <v>-0.5107531751786559</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -494,7 +494,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.541205784745187</v>
+        <v>0.659888126417628</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -502,7 +502,7 @@
         <v>128</v>
       </c>
       <c r="B4">
-        <v>0.8739268609724464</v>
+        <v>0.8284888105101889</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -514,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1789862695160596</v>
+        <v>-0.4669612063638096</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>4.298789582829578</v>
+        <v>0.6021435811555643</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -534,7 +534,7 @@
         <v>132</v>
       </c>
       <c r="B5">
-        <v>0.8834718259204246</v>
+        <v>0.8166713332729186</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.06212020846392313</v>
+        <v>-0.6440512652172118</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -558,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>-6.090105392067215</v>
+        <v>-0.9072544033899735</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -566,7 +566,7 @@
         <v>134</v>
       </c>
       <c r="B6">
-        <v>0.8101664739908526</v>
+        <v>0.7856463492376675</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>-0.03214084123039537</v>
+        <v>-0.3939408733220401</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>-0.5038026358534252</v>
+        <v>-0.6061675427787652</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -598,7 +598,7 @@
         <v>136</v>
       </c>
       <c r="B7">
-        <v>0.8315640236045749</v>
+        <v>0.7621859773132071</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -610,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>-0.05562104189304217</v>
+        <v>-0.3688413192581249</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -622,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>-0.6191585731671831</v>
+        <v>-0.592590661221202</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -630,7 +630,7 @@
         <v>138</v>
       </c>
       <c r="B8">
-        <v>0.8168772024058819</v>
+        <v>0.8167642621291933</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.1101486339057021</v>
+        <v>0.5060171112935425</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -654,7 +654,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.5320099225380904</v>
+        <v>0.604040810550924</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -662,7 +662,7 @@
         <v>144</v>
       </c>
       <c r="B9">
-        <v>0.7965653181829219</v>
+        <v>0.7298409743163429</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -674,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>-0.05901502738341916</v>
+        <v>-0.380952682856165</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>-2.053916095605086</v>
+        <v>-0.545852142808624</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -694,7 +694,7 @@
         <v>146</v>
       </c>
       <c r="B10">
-        <v>0.8463997298806604</v>
+        <v>0.7873838827589105</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -706,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.04400800582821683</v>
+        <v>0.3448784394287218</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -718,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>-0.2770106997326406</v>
+        <v>-0.6201922654759529</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -726,7 +726,7 @@
         <v>156</v>
       </c>
       <c r="B11">
-        <v>0.1457611398891636</v>
+        <v>0.1633157729489279</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>-0.03162174818731048</v>
+        <v>-0.4453151504741452</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -750,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.01679144935774508</v>
+        <v>0.3231813326375269</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -758,7 +758,7 @@
         <v>158</v>
       </c>
       <c r="B12">
-        <v>0.3900254692522015</v>
+        <v>0.5316860107187826</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>-0.02824567085497308</v>
+        <v>0.3867971054479267</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -782,7 +782,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.2291549375934149</v>
+        <v>0.6149070381258281</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -790,7 +790,7 @@
         <v>174</v>
       </c>
       <c r="B13">
-        <v>0.63232938354846</v>
+        <v>0.7099187301197926</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -802,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>-0.03357738728005554</v>
+        <v>-0.2911211630214038</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -814,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0.1966491891647955</v>
+        <v>0.706155190533714</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -822,7 +822,7 @@
         <v>182</v>
       </c>
       <c r="B14">
-        <v>0.7494941780320205</v>
+        <v>0.6860996232423073</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0.05077293796987024</v>
+        <v>0.3970651141398553</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -846,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0.3304542825645972</v>
+        <v>0.5746657963495071</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -854,7 +854,7 @@
         <v>184</v>
       </c>
       <c r="B15">
-        <v>0.7733853682364822</v>
+        <v>0.7099765534371616</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>-0.03873270488702656</v>
+        <v>-0.3072152285082598</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>-0.2400506303933087</v>
+        <v>-0.5426382720762762</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -886,7 +886,7 @@
         <v>186</v>
       </c>
       <c r="B16">
-        <v>0.2951174354571064</v>
+        <v>0.2853797359787679</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -898,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>-0.0494049166311059</v>
+        <v>-0.3796307755022347</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -910,7 +910,7 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>2.253967138089005</v>
+        <v>13.9510825385243</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -918,7 +918,7 @@
         <v>199</v>
       </c>
       <c r="B17">
-        <v>0.4663281872046415</v>
+        <v>0.4272290166072092</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0.03238548111488364</v>
+        <v>0.2232305707268276</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -942,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>-0.2992625195917438</v>
+        <v>-0.5573401192685299</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -950,7 +950,7 @@
         <v>228</v>
       </c>
       <c r="B18">
-        <v>0.1161107001140945</v>
+        <v>0.1348496652117076</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -962,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0.04359719820977784</v>
+        <v>0.4348570575493335</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>-0.2820016233720932</v>
+        <v>-0.6426493068944772</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -982,7 +982,7 @@
         <v>273</v>
       </c>
       <c r="B19">
-        <v>-0.03666643836248678</v>
+        <v>-0.05145976892022799</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>-0.2352706801736113</v>
+        <v>0.2912410106976744</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1006,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>4.499524608348935</v>
+        <v>-6.997510347546987</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1014,7 +1014,7 @@
         <v>534</v>
       </c>
       <c r="B20">
-        <v>0.2925785132178155</v>
+        <v>0.2831366615843744</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1026,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0.02883882494202798</v>
+        <v>0.2688418847798602</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1038,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>-0.2131234373914346</v>
+        <v>-0.5494584946267194</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1046,7 +1046,7 @@
         <v>542</v>
       </c>
       <c r="B21">
-        <v>0.04783831019918679</v>
+        <v>0.04648977929059236</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>-0.06356724193609851</v>
+        <v>-0.5152074001612627</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0.2129700722679557</v>
+        <v>0.3778642395909452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>